<commit_message>
bj: update bsa form
</commit_message>
<xml_diff>
--- a/ONCHO/Breeding Site Survey/Benin/bj_oncho_bsa_2_capture_form_202207.xlsx
+++ b/ONCHO/Breeding Site Survey/Benin/bj_oncho_bsa_2_capture_form_202207.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="12255" tabRatio="500" activeTab="2"/>
+    <workbookView windowWidth="28800" windowHeight="12255" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="440" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="443" uniqueCount="150">
   <si>
     <t>type</t>
   </si>
@@ -238,6 +238,9 @@
   </si>
   <si>
     <t>16:00 - 17:00</t>
+  </si>
+  <si>
+    <t>17:00 - 18:00</t>
   </si>
   <si>
     <t>weather_list</t>
@@ -470,9 +473,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="24">
@@ -507,9 +510,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -522,34 +525,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -568,8 +548,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -583,9 +564,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -599,7 +579,67 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -615,44 +655,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -673,25 +676,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -703,19 +694,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -733,13 +724,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -751,13 +748,91 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -769,61 +844,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -835,25 +856,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -930,6 +933,21 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top style="thin">
@@ -937,6 +955,15 @@
       </top>
       <bottom style="double">
         <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -955,175 +982,151 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="6" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="26" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="26" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1929,12 +1932,12 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E122"/>
+  <dimension ref="A1:E123"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" outlineLevelCol="4"/>
@@ -2073,18 +2076,18 @@
     </row>
     <row r="12" spans="1:3">
       <c r="A12" t="s">
+        <v>63</v>
+      </c>
+      <c r="B12" t="s">
         <v>74</v>
       </c>
-      <c r="B12" t="s">
-        <v>75</v>
-      </c>
       <c r="C12" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B13" t="s">
         <v>76</v>
@@ -2095,7 +2098,7 @@
     </row>
     <row r="14" spans="1:3">
       <c r="A14" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B14" t="s">
         <v>77</v>
@@ -2104,14 +2107,14 @@
         <v>77</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
-      <c r="A16" t="s">
-        <v>61</v>
-      </c>
-      <c r="B16" s="3" t="s">
+    <row r="15" spans="1:3">
+      <c r="A15" t="s">
+        <v>75</v>
+      </c>
+      <c r="B15" t="s">
         <v>78</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="C15" t="s">
         <v>78</v>
       </c>
     </row>
@@ -2155,7 +2158,7 @@
       <c r="B20" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C20" s="3" t="s">
         <v>82</v>
       </c>
     </row>
@@ -2335,18 +2338,15 @@
         <v>98</v>
       </c>
     </row>
-    <row r="38" spans="1:4">
-      <c r="A38" t="s">
-        <v>62</v>
-      </c>
-      <c r="B38" t="s">
+    <row r="37" spans="1:3">
+      <c r="A37" t="s">
+        <v>61</v>
+      </c>
+      <c r="B37" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="C38" t="s">
+      <c r="C37" t="s">
         <v>99</v>
-      </c>
-      <c r="D38" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="39" spans="1:4">
@@ -2360,7 +2360,7 @@
         <v>100</v>
       </c>
       <c r="D39" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="40" spans="1:4">
@@ -2388,7 +2388,7 @@
         <v>102</v>
       </c>
       <c r="D41" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="42" spans="1:4">
@@ -2416,7 +2416,7 @@
         <v>104</v>
       </c>
       <c r="D43" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="44" spans="1:4">
@@ -2430,7 +2430,7 @@
         <v>105</v>
       </c>
       <c r="D44" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="45" spans="1:4">
@@ -2458,7 +2458,7 @@
         <v>107</v>
       </c>
       <c r="D46" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="47" spans="1:4">
@@ -2486,7 +2486,7 @@
         <v>109</v>
       </c>
       <c r="D48" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="49" spans="1:4">
@@ -2500,7 +2500,7 @@
         <v>110</v>
       </c>
       <c r="D49" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="50" spans="1:4">
@@ -2542,7 +2542,7 @@
         <v>113</v>
       </c>
       <c r="D52" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="53" spans="1:4">
@@ -2584,7 +2584,7 @@
         <v>116</v>
       </c>
       <c r="D55" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="56" spans="1:4">
@@ -2598,7 +2598,7 @@
         <v>117</v>
       </c>
       <c r="D56" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="57" spans="1:4">
@@ -2654,7 +2654,7 @@
         <v>121</v>
       </c>
       <c r="D60" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="61" spans="1:4">
@@ -2696,7 +2696,7 @@
         <v>124</v>
       </c>
       <c r="D63" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="64" spans="1:4">
@@ -2738,7 +2738,7 @@
         <v>127</v>
       </c>
       <c r="D66" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="67" spans="1:4">
@@ -2766,7 +2766,7 @@
         <v>129</v>
       </c>
       <c r="D68" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="69" spans="1:4">
@@ -2780,7 +2780,7 @@
         <v>130</v>
       </c>
       <c r="D69" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="70" spans="1:4">
@@ -2808,7 +2808,7 @@
         <v>132</v>
       </c>
       <c r="D71" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="72" spans="1:4">
@@ -2836,7 +2836,7 @@
         <v>134</v>
       </c>
       <c r="D73" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="74" spans="1:4">
@@ -2850,7 +2850,7 @@
         <v>135</v>
       </c>
       <c r="D74" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="75" spans="1:4">
@@ -2864,7 +2864,7 @@
         <v>136</v>
       </c>
       <c r="D75" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="76" spans="1:4">
@@ -2878,7 +2878,7 @@
         <v>137</v>
       </c>
       <c r="D76" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="77" spans="1:4">
@@ -2920,32 +2920,32 @@
         <v>140</v>
       </c>
       <c r="D79" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="81" spans="1:5">
-      <c r="A81" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4">
+      <c r="A80" t="s">
+        <v>62</v>
+      </c>
+      <c r="B80" t="s">
         <v>141</v>
       </c>
-      <c r="B81">
-        <v>101</v>
-      </c>
-      <c r="C81">
-        <v>101</v>
-      </c>
-      <c r="E81" t="s">
-        <v>106</v>
+      <c r="C80" t="s">
+        <v>141</v>
+      </c>
+      <c r="D80" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="82" spans="1:5">
       <c r="A82" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B82">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C82">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E82" t="s">
         <v>107</v>
@@ -2953,27 +2953,27 @@
     </row>
     <row r="83" spans="1:5">
       <c r="A83" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B83">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C83">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E83" t="s">
-        <v>120</v>
+        <v>108</v>
       </c>
     </row>
     <row r="84" spans="1:5">
       <c r="A84" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B84">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C84">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E84" t="s">
         <v>121</v>
@@ -2981,69 +2981,69 @@
     </row>
     <row r="85" spans="1:5">
       <c r="A85" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B85">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C85">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E85" t="s">
-        <v>138</v>
+        <v>122</v>
       </c>
     </row>
     <row r="86" spans="1:5">
       <c r="A86" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B86">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C86">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E86" t="s">
-        <v>118</v>
+        <v>139</v>
       </c>
     </row>
     <row r="87" spans="1:5">
       <c r="A87" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B87">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C87">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E87" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
     </row>
     <row r="88" spans="1:5">
       <c r="A88" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B88">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C88">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E88" t="s">
-        <v>112</v>
+        <v>126</v>
       </c>
     </row>
     <row r="89" spans="1:5">
       <c r="A89" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B89">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C89">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E89" t="s">
         <v>113</v>
@@ -3051,41 +3051,41 @@
     </row>
     <row r="90" spans="1:5">
       <c r="A90" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B90">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C90">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E90" t="s">
-        <v>105</v>
+        <v>114</v>
       </c>
     </row>
     <row r="91" spans="1:5">
       <c r="A91" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B91">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C91">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E91" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
     </row>
     <row r="92" spans="1:5">
       <c r="A92" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B92">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C92">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E92" t="s">
         <v>104</v>
@@ -3093,69 +3093,69 @@
     </row>
     <row r="93" spans="1:5">
       <c r="A93" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B93">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C93">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E93" t="s">
-        <v>124</v>
+        <v>105</v>
       </c>
     </row>
     <row r="94" spans="1:5">
       <c r="A94" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B94">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C94">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E94" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
     </row>
     <row r="95" spans="1:5">
       <c r="A95" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B95">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C95">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E95" t="s">
-        <v>137</v>
+        <v>124</v>
       </c>
     </row>
     <row r="96" spans="1:5">
       <c r="A96" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B96">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C96">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E96" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
     </row>
     <row r="97" spans="1:5">
       <c r="A97" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B97">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C97">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E97" t="s">
         <v>136</v>
@@ -3163,27 +3163,27 @@
     </row>
     <row r="98" spans="1:5">
       <c r="A98" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B98">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C98">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E98" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
     </row>
     <row r="99" spans="1:5">
       <c r="A99" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B99">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C99">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E99" t="s">
         <v>134</v>
@@ -3191,27 +3191,27 @@
     </row>
     <row r="100" spans="1:5">
       <c r="A100" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B100">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C100">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E100" t="s">
-        <v>101</v>
+        <v>135</v>
       </c>
     </row>
     <row r="101" spans="1:5">
       <c r="A101" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B101">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C101">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E101" t="s">
         <v>102</v>
@@ -3219,41 +3219,41 @@
     </row>
     <row r="102" spans="1:5">
       <c r="A102" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B102">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C102">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E102" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
     </row>
     <row r="103" spans="1:5">
       <c r="A103" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B103">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C103">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E103" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
     </row>
     <row r="104" spans="1:5">
       <c r="A104" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B104">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C104">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E104" t="s">
         <v>109</v>
@@ -3261,27 +3261,27 @@
     </row>
     <row r="105" spans="1:5">
       <c r="A105" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B105">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C105">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E105" t="s">
-        <v>126</v>
+        <v>110</v>
       </c>
     </row>
     <row r="106" spans="1:5">
       <c r="A106" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B106">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C106">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E106" t="s">
         <v>127</v>
@@ -3289,13 +3289,13 @@
     </row>
     <row r="107" spans="1:5">
       <c r="A107" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B107">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C107">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E107" t="s">
         <v>128</v>
@@ -3303,55 +3303,55 @@
     </row>
     <row r="108" spans="1:5">
       <c r="A108" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B108">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C108">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E108" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="109" spans="1:5">
       <c r="A109" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B109">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C109">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E109" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
     </row>
     <row r="110" spans="1:5">
       <c r="A110" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B110">
+        <v>129</v>
+      </c>
+      <c r="C110">
+        <v>129</v>
+      </c>
+      <c r="E110" t="s">
         <v>130</v>
-      </c>
-      <c r="C110">
-        <v>130</v>
-      </c>
-      <c r="E110" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="111" spans="1:5">
       <c r="A111" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B111">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C111">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E111" t="s">
         <v>132</v>
@@ -3359,27 +3359,27 @@
     </row>
     <row r="112" spans="1:5">
       <c r="A112" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B112">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C112">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E112" t="s">
-        <v>116</v>
+        <v>133</v>
       </c>
     </row>
     <row r="113" spans="1:5">
       <c r="A113" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B113">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C113">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E113" t="s">
         <v>117</v>
@@ -3387,69 +3387,69 @@
     </row>
     <row r="114" spans="1:5">
       <c r="A114" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B114">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C114">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E114" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
     </row>
     <row r="115" spans="1:5">
       <c r="A115" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B115">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C115">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E115" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
     </row>
     <row r="116" spans="1:5">
       <c r="A116" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B116">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C116">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E116" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
     </row>
     <row r="117" spans="1:5">
       <c r="A117" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B117">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C117">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E117" t="s">
-        <v>99</v>
+        <v>120</v>
       </c>
     </row>
     <row r="118" spans="1:5">
       <c r="A118" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B118">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C118">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E118" t="s">
         <v>100</v>
@@ -3457,58 +3457,72 @@
     </row>
     <row r="119" spans="1:5">
       <c r="A119" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B119">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C119">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E119" t="s">
-        <v>114</v>
+        <v>101</v>
       </c>
     </row>
     <row r="120" spans="1:5">
       <c r="A120" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B120">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C120">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E120" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
     </row>
     <row r="121" spans="1:5">
       <c r="A121" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B121">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C121">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E121" t="s">
-        <v>140</v>
+        <v>112</v>
       </c>
     </row>
     <row r="122" spans="1:5">
       <c r="A122" t="s">
+        <v>142</v>
+      </c>
+      <c r="B122">
         <v>141</v>
       </c>
-      <c r="B122">
-        <v>142</v>
-      </c>
       <c r="C122">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E122" t="s">
-        <v>139</v>
+        <v>141</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5">
+      <c r="A123" t="s">
+        <v>142</v>
+      </c>
+      <c r="B123">
+        <v>142</v>
+      </c>
+      <c r="C123">
+        <v>142</v>
+      </c>
+      <c r="E123" t="s">
+        <v>140</v>
       </c>
     </row>
   </sheetData>
@@ -3526,7 +3540,7 @@
   <sheetPr/>
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -3538,27 +3552,27 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="3" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B2" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="C2" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="D2" t="s">
         <v>20</v>

</xml_diff>